<commit_message>
some agents and some small changes
</commit_message>
<xml_diff>
--- a/agents/Othello/csv/multiTrain-lambda.xlsx
+++ b/agents/Othello/csv/multiTrain-lambda.xlsx
@@ -13,13 +13,17 @@
   </bookViews>
   <sheets>
     <sheet name="multiTrain-lambda" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="horizonCut">Tabelle1!$D$5</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>TDNTuple3Agt: USESYM:true, P:4, NORMALIZE:false, sigmoid:tanh, lambda:0.9, horizon:44, AFTERSTATE:false, learnFromRM: false</t>
   </si>
@@ -53,13 +57,19 @@
   <si>
     <t>lambda</t>
   </si>
+  <si>
+    <t>horizonCut</t>
+  </si>
+  <si>
+    <t>horizon</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -540,7 +550,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -865,7 +875,7 @@
   <dimension ref="A1:I1253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:I1253"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38412,4 +38422,125 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>1E-4</v>
+      </c>
+      <c r="D8">
+        <f>ROUND(LN(horizonCut)/LN(C8)+0.5,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>0.1</v>
+      </c>
+      <c r="D9">
+        <f>ROUND(LN(horizonCut)/LN(C9)+0.5,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>0.2</v>
+      </c>
+      <c r="D10">
+        <f>ROUND(LN(horizonCut)/LN(C10)+0.5,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>0.3</v>
+      </c>
+      <c r="D11">
+        <f>ROUND(LN(horizonCut)/LN(C11)+0.5,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>0.4</v>
+      </c>
+      <c r="D12">
+        <f>ROUND(LN(horizonCut)/LN(C12)+0.5,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>0.5</v>
+      </c>
+      <c r="D13">
+        <f>ROUND(LN(horizonCut)/LN(C13)+0.5,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>0.6</v>
+      </c>
+      <c r="D14">
+        <f>ROUND(LN(horizonCut)/LN(C14)+0.5,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>0.7</v>
+      </c>
+      <c r="D15">
+        <f>ROUND(LN(horizonCut)/LN(C15)+0.5,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>0.8</v>
+      </c>
+      <c r="D16">
+        <f>ROUND(LN(horizonCut)/LN(C16)+0.5,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>0.9</v>
+      </c>
+      <c r="D17">
+        <f>ROUND(LN(horizonCut)/LN(C17)+0.5,0)</f>
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>